<commit_message>
complte tool fill form irs
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9898,6 +9898,422 @@
         </is>
       </c>
     </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>33-4000359</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>BLUESKY INNOVATIONS LLC</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>432813777</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Basilia</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Gonzalez</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>1992-01-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>1828 James Street</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>Irving</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>75061</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>33-4000640</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>STELLARPEAK VENTURES LLC</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>099664210</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>RAFAEL</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>PEREZ-ESPEJO</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>1958-10-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>1100 GOUGH ST</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>SAN FRANCISCO</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>94109</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>33-4000781</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>NEXUSFLOW TECHNOLOGIES LLC</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>643015000</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>ZACHARY</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>DAVIDSON</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>1980-09-17 00:00:00</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>955 PINE STREET</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>SAN FRANCISCO</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>94108</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>33-4000836</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>APEXVIBE GLOBAL LLC</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>625247624</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>JOSHUA</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>BONGAWIL</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>1988-11-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>236 SAGEBRUSH LANE</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>AMERICAN CANYON</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>94503</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>33-4000904</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>HORIZONWAVE INDUSTRIES LLC</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>620425729</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>ARACELI</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>MARTIN</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>1990-01-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>190 HALE ST</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>SAN FRANCISCO</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>94134</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>33-4000992</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>REDSTONE STRATEGIES LLC</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>615361434</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>HARMONIE</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>WONG</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>1990-03-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>42 BERKELEY WAY</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>SAN FRANCISCO</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>94131</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>33-4001063</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>NOVACRAFT HOLDINGS LLC</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>612407257</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>JENNY</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>VALDEZ</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>1988-03-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>990 MAGNOLIA AVE</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>MILLBRAE</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>94030</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>33-4001534</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>CRYSTALCOVE ENTERPRISES LLC</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>630045084</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>AVIYANCA</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>PRAKASH</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>1993-11-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>711 TORREYA AVENUE</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>SUNNYVALE</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>94086</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>